<commit_message>
Add population chart for the very old
</commit_message>
<xml_diff>
--- a/data/ons-population/explore/mortality_rates.xlsx
+++ b/data/ons-population/explore/mortality_rates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\projects\work\covid-stats\data\ons-population\explore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBE73D9-1468-46E4-8B64-1799F8C38A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8022E3C1-AF58-4836-84B7-18BB9EEC49EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8A80DE31-D447-4B3A-90FE-EC624D4C6966}"/>
   </bookViews>
@@ -7060,6 +7060,523 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>UK Population Aged 90+ mid-2020</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>Based on 2020 mid-year</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t> population estimates (ONS)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2020'!$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UK mid-year population estimate 2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'2020'!$A$96:$A$111</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2020'!$E$96:$E$111</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>139390</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>112650</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90030</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72270</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56330</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42520</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31320</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22560</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16090</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7590</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1790</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>790</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5268-4120-ACCF-80329D07DFAC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="550227856"/>
+        <c:axId val="550231136"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="550227856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Age</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="550231136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="5"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="550231136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Persons</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="550227856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7791,6 +8308,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -11313,6 +11870,509 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12072,6 +13132,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5741876-C36A-4212-B007-967969252DAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -12421,10 +13519,10 @@
   <dimension ref="A1:N121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="L66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="K84" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AJ75" sqref="AJ75"/>
+      <selection pane="bottomRight" activeCell="AA115" sqref="AA115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15835,7 +16933,7 @@
         <v>31437.783281249998</v>
       </c>
       <c r="K70" s="7">
-        <f t="shared" ref="K70:M106" si="18">J70*($A70+0.5)</f>
+        <f t="shared" ref="K70:M104" si="18">J70*($A70+0.5)</f>
         <v>2027737.0216406249</v>
       </c>
       <c r="L70" s="7">
@@ -15878,7 +16976,7 @@
         <v>13160.856088200002</v>
       </c>
       <c r="I71" s="7">
-        <f t="shared" ref="I71:I106" si="22">H71*($A71+0.5)</f>
+        <f t="shared" ref="I71:I104" si="22">H71*($A71+0.5)</f>
         <v>862036.07377710007</v>
       </c>
       <c r="J71" s="7">
@@ -17451,7 +18549,7 @@
         <v>8327.4931439999982</v>
       </c>
       <c r="G102" s="7">
-        <f t="shared" ref="G102:G106" si="23">F102*(A102+0.5)</f>
+        <f t="shared" ref="G102:G104" si="23">F102*(A102+0.5)</f>
         <v>803603.08839599986</v>
       </c>
       <c r="H102" s="7">

</xml_diff>

<commit_message>
Checkin saved file - maybe not changed
</commit_message>
<xml_diff>
--- a/data/ons-population/explore/mortality_rates.xlsx
+++ b/data/ons-population/explore/mortality_rates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\projects\work\covid-stats\data\ons-population\explore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8022E3C1-AF58-4836-84B7-18BB9EEC49EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1A6654-3774-4A4E-A376-F3FAE9BD9438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8A80DE31-D447-4B3A-90FE-EC624D4C6966}"/>
   </bookViews>
@@ -13519,10 +13519,10 @@
   <dimension ref="A1:N121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="K84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AA115" sqref="AA115"/>
+      <selection pane="bottomRight" activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>